<commit_message>
Update Residual anomalies document.
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_CommLib_Android_JaiVis-20161118-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_CommLib_Android_JaiVis-20161118-01V01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="689" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="689" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="93">
   <si>
     <t>1.1</t>
   </si>
@@ -354,9 +354,6 @@
     <t>JaiVis-20161118-01V01</t>
   </si>
   <si>
-    <t>2016-NOV-18</t>
-  </si>
-  <si>
     <t>Jaime Visser</t>
   </si>
   <si>
@@ -401,48 +398,56 @@
     <t>Document creation, and new release</t>
   </si>
   <si>
+    <t>COM-191</t>
+  </si>
+  <si>
+    <t>Cannot related failed requests to original requests in case of queueing</t>
+  </si>
+  <si>
+    <t>COM-83</t>
+  </si>
+  <si>
+    <t>Small legal issue, format of copyright notice in code is incorrect</t>
+  </si>
+  <si>
+    <t>COM-13</t>
+  </si>
+  <si>
+    <t>SampleApp does not switch from local to remote requests (and vice versa)</t>
+  </si>
+  <si>
+    <t>COM-7</t>
+  </si>
+  <si>
+    <t>Register Protocol Addresses Request Android</t>
+  </si>
+  <si>
+    <t>COM-5</t>
+  </si>
+  <si>
+    <t>Push notification languages are not updated when locale changes</t>
+  </si>
+  <si>
+    <t>COM-4</t>
+  </si>
+  <si>
+    <t>Connect screen shows devices that actually are not present on the local network</t>
+  </si>
+  <si>
+    <t>Document creation, and update for release 2.0.0</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Document creation, and update for release </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;release id&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Conclusion: The build </t>
+      <t>Conclusion: The build can be released becaus</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>&lt;can/cannot&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> be released because </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;reason&gt;</t>
+      <t>e there are no major anomalies</t>
     </r>
     <r>
       <rPr>
@@ -454,47 +459,26 @@
     </r>
   </si>
   <si>
-    <t>COM-191</t>
-  </si>
-  <si>
-    <t>Cannot related failed requests to original requests in case of queueing</t>
-  </si>
-  <si>
-    <t>COM-83</t>
-  </si>
-  <si>
-    <t>Small legal issue, format of copyright notice in code is incorrect</t>
-  </si>
-  <si>
-    <t>COM-13</t>
-  </si>
-  <si>
-    <t>SampleApp does not switch from local to remote requests (and vice versa)</t>
-  </si>
-  <si>
-    <t>COM-7</t>
-  </si>
-  <si>
-    <t>Register Protocol Addresses Request Android</t>
-  </si>
-  <si>
-    <t>COM-5</t>
-  </si>
-  <si>
-    <t>Push notification languages are not updated when locale changes</t>
-  </si>
-  <si>
-    <t>COM-4</t>
-  </si>
-  <si>
-    <t>Connect screen shows devices that actually are not present on the local network</t>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>2016-Dec-01</t>
+  </si>
+  <si>
+    <t>Update after review comment</t>
+  </si>
+  <si>
+    <t>Review comments</t>
+  </si>
+  <si>
+    <t>2016-DEC-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,12 +751,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -830,7 +808,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1085,6 +1063,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1093,7 +1084,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1374,6 +1365,10 @@
     <xf numFmtId="0" fontId="37" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2306,8 +2301,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:F7" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
-  <autoFilter ref="B6:F7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:F8" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="B6:F8"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Version"/>
     <tableColumn id="2" name="Date" dataDxfId="1"/>
@@ -2612,7 +2607,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2631,7 +2626,7 @@
         <v>43</v>
       </c>
       <c r="B1" s="60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -2696,7 +2691,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="102" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
@@ -2748,17 +2743,17 @@
         <v>13</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="105"/>
       <c r="F13" s="28" t="s">
         <v>17</v>
       </c>
       <c r="G13" s="61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2766,7 +2761,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="D14" s="105"/>
       <c r="E14" s="105"/>
@@ -2862,7 +2857,7 @@
   <sheetData>
     <row r="1" spans="2:6" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="6"/>
       <c r="E1" s="6"/>
@@ -2897,7 +2892,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="112" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="113"/>
       <c r="F6" s="114"/>
@@ -2910,7 +2905,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="115" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="115"/>
       <c r="F7" s="115"/>
@@ -3080,7 +3075,7 @@
   <dimension ref="B1:N179"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3096,7 +3091,7 @@
   <sheetData>
     <row r="1" spans="2:14" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -3182,16 +3177,16 @@
         <v>45</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="61" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="F7" s="89" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
@@ -3202,12 +3197,22 @@
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B8" s="100"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
+    <row r="8" spans="2:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="B8" s="135" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="136" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="136" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="135" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="135" t="s">
+        <v>91</v>
+      </c>
       <c r="G8" s="100"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
@@ -5819,7 +5824,7 @@
   <sheetData>
     <row r="1" spans="2:37" s="34" customFormat="1" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="35"/>
       <c r="E1" s="36"/>
@@ -6137,8 +6142,8 @@
   </sheetPr>
   <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6850,7 +6855,7 @@
   <sheetData>
     <row r="1" spans="2:4" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6898,7 +6903,7 @@
         <v>51</v>
       </c>
       <c r="C8" s="82">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8" s="37"/>
     </row>
@@ -6907,7 +6912,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="84">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" s="39"/>
     </row>
@@ -6918,7 +6923,7 @@
     </row>
     <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="38" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -6951,8 +6956,8 @@
   </sheetPr>
   <dimension ref="B1:AH29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7663,7 +7668,7 @@
   <sheetData>
     <row r="1" spans="2:34" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:34" ht="35" customHeight="1" x14ac:dyDescent="0.15">
@@ -7687,10 +7692,10 @@
     </row>
     <row r="4" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="94" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4" s="95" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" s="69" t="s">
         <v>52</v>
@@ -7703,10 +7708,10 @@
     </row>
     <row r="5" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="94" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C5" s="95" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D5" s="69" t="s">
         <v>52</v>
@@ -7719,10 +7724,10 @@
     </row>
     <row r="6" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="94" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C6" s="95" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D6" s="69" t="s">
         <v>51</v>
@@ -7735,10 +7740,10 @@
     </row>
     <row r="7" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="94" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D7" s="69" t="s">
         <v>51</v>
@@ -7751,10 +7756,10 @@
     </row>
     <row r="8" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="94" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C8" s="95" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D8" s="69" t="s">
         <v>51</v>
@@ -7767,10 +7772,10 @@
     </row>
     <row r="9" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" s="94" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C9" s="95" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D9" s="69" t="s">
         <v>51</v>
@@ -7915,52 +7920,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <View_x0020_CRM xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_CRM>
-    <View_x0020_Qua xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Qua>
-    <Document_x0020_author xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
-      <UserInfo>
-        <DisplayName>Jacobs, Frans</DisplayName>
-        <AccountId>1</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </Document_x0020_author>
-    <Document_x0020_type xmlns="5db227b6-3c56-4158-ad71-bd648583e357">Template</Document_x0020_type>
-    <View_x0020_Eng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_Eng>
-    <View_x0020_Production xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</View_x0020_Production>
-    <Relevant_x0020_to_x0020_ISO_x0020_13485 xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Relevant_x0020_to_x0020_ISO_x0020_13485>
-    <PInS_x0020_department xmlns="5db227b6-3c56-4158-ad71-bd648583e357">140 Software</PInS_x0020_department>
-    <Doc_x0020_nr. xmlns="5db227b6-3c56-4158-ad71-bd648583e357">BMS-REA-719</Doc_x0020_nr.>
-    <DLCPolicyLabelLock xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a" xsi:nil="true"/>
-    <Linked_x0020_to_x0020_PQRS xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</Linked_x0020_to_x0020_PQRS>
-    <Safety_x0020_relevant xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Safety_x0020_relevant>
-    <Approver xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
-      <UserInfo>
-        <DisplayName>Jacobs, Frans</DisplayName>
-        <AccountId>1</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </Approver>
-    <Reviewers xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Reviewers>
-    <Process xmlns="5db227b6-3c56-4158-ad71-bd648583e357">04 Realisation</Process>
-    <View_x0020_PL xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_PL>
-    <View_x0020_Mng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Mng>
-    <DLCPolicyLabelClientValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">{_UIVersionString}
-{_ModerationStatus}</DLCPolicyLabelClientValue>
-    <DLCPolicyLabelValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">1.0
-Approved</DLCPolicyLabelValue>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="02 Departmental document" ma:contentTypeID="0x0101001E9AF57F6A6FB1498E6BAB1704371DB9020048B3E13A56EC2B4880B8E17388254DB6" ma:contentTypeVersion="42" ma:contentTypeDescription="A document under departmental control" ma:contentTypeScope="" ma:versionID="28e15f56482d8af7e67347cbef2a0996">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5db227b6-3c56-4158-ad71-bd648583e357" xmlns:ns3="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa83b77159cc0e9c22a0bfa7b50ba950" ns2:_="" ns3:_="">
     <xsd:import namespace="5db227b6-3c56-4158-ad71-bd648583e357"/>
@@ -8350,7 +8309,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <p:Policy xmlns:p="office.server.policy" id="" local="true">
   <p:Name>02 Departmental document</p:Name>
@@ -8372,7 +8331,7 @@
 </p:Policy>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8381,24 +8340,53 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1320B1-D764-4C81-9B48-5F60482C3805}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5db227b6-3c56-4158-ad71-bd648583e357"/>
-    <ds:schemaRef ds:uri="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <View_x0020_CRM xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_CRM>
+    <View_x0020_Qua xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Qua>
+    <Document_x0020_author xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
+      <UserInfo>
+        <DisplayName>Jacobs, Frans</DisplayName>
+        <AccountId>1</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </Document_x0020_author>
+    <Document_x0020_type xmlns="5db227b6-3c56-4158-ad71-bd648583e357">Template</Document_x0020_type>
+    <View_x0020_Eng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_Eng>
+    <View_x0020_Production xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</View_x0020_Production>
+    <Relevant_x0020_to_x0020_ISO_x0020_13485 xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Relevant_x0020_to_x0020_ISO_x0020_13485>
+    <PInS_x0020_department xmlns="5db227b6-3c56-4158-ad71-bd648583e357">140 Software</PInS_x0020_department>
+    <Doc_x0020_nr. xmlns="5db227b6-3c56-4158-ad71-bd648583e357">BMS-REA-719</Doc_x0020_nr.>
+    <DLCPolicyLabelLock xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a" xsi:nil="true"/>
+    <Linked_x0020_to_x0020_PQRS xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</Linked_x0020_to_x0020_PQRS>
+    <Safety_x0020_relevant xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Safety_x0020_relevant>
+    <Approver xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
+      <UserInfo>
+        <DisplayName>Jacobs, Frans</DisplayName>
+        <AccountId>1</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </Approver>
+    <Reviewers xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Reviewers>
+    <Process xmlns="5db227b6-3c56-4158-ad71-bd648583e357">04 Realisation</Process>
+    <View_x0020_PL xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_PL>
+    <View_x0020_Mng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Mng>
+    <DLCPolicyLabelClientValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">{_UIVersionString}
+{_ModerationStatus}</DLCPolicyLabelClientValue>
+    <DLCPolicyLabelValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">1.0
+Approved</DLCPolicyLabelValue>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3331877D-A973-4A26-8E19-E1DD744074D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8417,7 +8405,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E0ECFB5-0E65-4944-A2C3-A12752EA8F83}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="office.server.policy"/>
@@ -8425,10 +8413,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F20991C-9C75-4A23-AD56-83877EA734AB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1320B1-D764-4C81-9B48-5F60482C3805}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="5db227b6-3c56-4158-ad71-bd648583e357"/>
+    <ds:schemaRef ds:uri="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update colour coding on anomalies tab.
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_CommLib_Android_JaiVis-20161118-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_CommLib_Android_JaiVis-20161118-01V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="689" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="689" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -1298,6 +1298,10 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1365,10 +1369,6 @@
     <xf numFmtId="0" fontId="37" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2657,11 +2657,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -2727,10 +2727,10 @@
       <c r="C12" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="104" t="s">
+      <c r="D12" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="104"/>
+      <c r="E12" s="106"/>
       <c r="F12" s="28" t="s">
         <v>16</v>
       </c>
@@ -2745,10 +2745,10 @@
       <c r="C13" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="105" t="s">
+      <c r="D13" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="105"/>
+      <c r="E13" s="107"/>
       <c r="F13" s="28" t="s">
         <v>17</v>
       </c>
@@ -2763,8 +2763,8 @@
       <c r="C14" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
       <c r="F14" s="28" t="s">
         <v>18</v>
       </c>
@@ -2891,11 +2891,11 @@
       <c r="C6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="112" t="s">
+      <c r="D6" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="113"/>
-      <c r="F6" s="114"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="116"/>
     </row>
     <row r="7" spans="2:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="30" t="s">
@@ -2904,11 +2904,11 @@
       <c r="C7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="115" t="s">
+      <c r="D7" s="117" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="115"/>
-      <c r="F7" s="115"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="117"/>
     </row>
     <row r="8" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="31" t="s">
@@ -2960,27 +2960,27 @@
       <c r="D12" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="116" t="s">
+      <c r="E12" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="116"/>
+      <c r="F12" s="118"/>
     </row>
     <row r="13" spans="2:6" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="31"/>
       <c r="D13" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="106" t="s">
+      <c r="E13" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="107"/>
+      <c r="F13" s="109"/>
     </row>
     <row r="14" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="32"/>
       <c r="C14" s="30"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="108"/>
-      <c r="F14" s="109"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="111"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
@@ -2993,8 +2993,8 @@
       <c r="B16" s="19"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="111"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="113"/>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="48"/>
@@ -3198,19 +3198,19 @@
       <c r="N7" s="17"/>
     </row>
     <row r="8" spans="2:14" ht="14" x14ac:dyDescent="0.15">
-      <c r="B8" s="135" t="s">
+      <c r="B8" s="103" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="136" t="s">
+      <c r="C8" s="104" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="136" t="s">
+      <c r="D8" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="135" t="s">
+      <c r="E8" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="135" t="s">
+      <c r="F8" s="103" t="s">
         <v>91</v>
       </c>
       <c r="G8" s="100"/>
@@ -5914,19 +5914,19 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:37" ht="120.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="125" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="124"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126"/>
     </row>
     <row r="5" spans="2:37" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="45"/>
@@ -5945,29 +5945,29 @@
       <c r="B6" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="125" t="s">
+      <c r="C6" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="127"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="129"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B7" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="128" t="s">
+      <c r="C7" s="130" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="129"/>
-      <c r="I7" s="130"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="132"/>
       <c r="M7" s="51"/>
       <c r="N7" s="51"/>
       <c r="O7" s="51"/>
@@ -5978,15 +5978,15 @@
       <c r="B8" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="133" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
-      <c r="H8" s="132"/>
-      <c r="I8" s="133"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="134"/>
+      <c r="I8" s="135"/>
       <c r="M8" s="51"/>
       <c r="N8" s="51"/>
       <c r="O8" s="51"/>
@@ -5997,15 +5997,15 @@
       <c r="B9" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="120" t="s">
+      <c r="C9" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="121"/>
-      <c r="E9" s="121"/>
-      <c r="F9" s="121"/>
-      <c r="G9" s="121"/>
-      <c r="H9" s="121"/>
-      <c r="I9" s="122"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="124"/>
       <c r="M9" s="51"/>
       <c r="N9" s="51"/>
       <c r="O9" s="51"/>
@@ -6030,15 +6030,15 @@
       <c r="B11" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="117" t="s">
+      <c r="C11" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="119"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="121"/>
     </row>
     <row r="12" spans="2:37" ht="18" x14ac:dyDescent="0.2">
       <c r="C12" s="64"/>
@@ -6142,8 +6142,8 @@
   </sheetPr>
   <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6860,11 +6860,11 @@
     </row>
     <row r="2" spans="2:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="2:4" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="134" t="s">
+      <c r="B3" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="37"/>
@@ -6956,8 +6956,8 @@
   </sheetPr>
   <dimension ref="B1:AH29"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7690,14 +7690,14 @@
       <c r="AG3" s="34"/>
       <c r="AH3" s="34"/>
     </row>
-    <row r="4" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:34" ht="16" x14ac:dyDescent="0.15">
       <c r="B4" s="94" t="s">
         <v>74</v>
       </c>
       <c r="C4" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="84" t="s">
         <v>52</v>
       </c>
       <c r="AD4" s="34"/>
@@ -7706,14 +7706,14 @@
       <c r="AG4" s="34"/>
       <c r="AH4" s="34"/>
     </row>
-    <row r="5" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:34" ht="16" x14ac:dyDescent="0.15">
       <c r="B5" s="94" t="s">
         <v>76</v>
       </c>
       <c r="C5" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="84" t="s">
         <v>52</v>
       </c>
       <c r="AD5" s="34"/>

</xml_diff>

<commit_message>
Fixes by Bas Flaton
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_CommLib_Android_JaiVis-20161118-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_CommLib_Android_JaiVis-20161118-01V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17460" tabRatio="689" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17460" tabRatio="689"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -465,9 +465,6 @@
     <t>Review comments</t>
   </si>
   <si>
-    <t>2016-DEC-01</t>
-  </si>
-  <si>
     <t>2016-Dec-13</t>
   </si>
   <si>
@@ -484,6 +481,9 @@
   </si>
   <si>
     <t>approved</t>
+  </si>
+  <si>
+    <t>2016-DEC-13</t>
   </si>
 </sst>
 </file>
@@ -1314,6 +1314,14 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1381,14 +1389,6 @@
     <xf numFmtId="0" fontId="37" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2626,8 +2626,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2677,11 +2677,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="105"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -2747,10 +2747,10 @@
       <c r="C12" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="106" t="s">
+      <c r="D12" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="106"/>
+      <c r="E12" s="110"/>
       <c r="F12" s="28" t="s">
         <v>16</v>
       </c>
@@ -2763,12 +2763,12 @@
         <v>13</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="107" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="107"/>
+      <c r="E13" s="111"/>
       <c r="F13" s="28" t="s">
         <v>17</v>
       </c>
@@ -2780,11 +2780,11 @@
       <c r="B14" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="140" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="107"/>
-      <c r="E14" s="107"/>
+      <c r="C14" s="108" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="111"/>
+      <c r="E14" s="111"/>
       <c r="F14" s="28" t="s">
         <v>18</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="61" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>34</v>
@@ -2842,7 +2842,8 @@
   <pageSetup paperSize="9" scale="76" fitToHeight="100" orientation="landscape" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.1&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F
+Version 1.0&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId3"/>
   <extLst>
@@ -2911,11 +2912,11 @@
       <c r="C6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="114" t="s">
+      <c r="D6" s="118" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="115"/>
-      <c r="F6" s="116"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="120"/>
     </row>
     <row r="7" spans="2:6" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
@@ -2924,11 +2925,11 @@
       <c r="C7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="117" t="s">
+      <c r="D7" s="121" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
     </row>
     <row r="8" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="31" t="s">
@@ -2980,27 +2981,27 @@
       <c r="D12" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="118" t="s">
+      <c r="E12" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="118"/>
+      <c r="F12" s="122"/>
     </row>
     <row r="13" spans="2:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="31"/>
       <c r="D13" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="108" t="s">
+      <c r="E13" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="109"/>
+      <c r="F13" s="113"/>
     </row>
     <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="32"/>
       <c r="C14" s="30"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="111"/>
+      <c r="E14" s="114"/>
+      <c r="F14" s="115"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
@@ -3013,8 +3014,8 @@
       <c r="B16" s="19"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="112"/>
-      <c r="F16" s="113"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="117"/>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="48"/>
@@ -3094,8 +3095,8 @@
   </sheetPr>
   <dimension ref="B1:N179"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3243,20 +3244,20 @@
       <c r="N8" s="17"/>
     </row>
     <row r="9" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B9" s="138" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="137" t="s">
+      <c r="B9" s="106" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="137" t="s">
+      <c r="E9" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="139" t="s">
+      <c r="F9" s="107" t="s">
         <v>94</v>
-      </c>
-      <c r="F9" s="139" t="s">
-        <v>95</v>
       </c>
       <c r="G9" s="100"/>
       <c r="H9" s="17"/>
@@ -5944,19 +5945,19 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:37" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="130"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="130"/>
     </row>
     <row r="5" spans="2:37" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="45"/>
@@ -5975,29 +5976,29 @@
       <c r="B6" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="127" t="s">
+      <c r="C6" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="129"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="133"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B7" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="130" t="s">
+      <c r="C7" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="131"/>
-      <c r="E7" s="131"/>
-      <c r="F7" s="131"/>
-      <c r="G7" s="131"/>
-      <c r="H7" s="131"/>
-      <c r="I7" s="132"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+      <c r="I7" s="136"/>
       <c r="M7" s="51"/>
       <c r="N7" s="51"/>
       <c r="O7" s="51"/>
@@ -6008,15 +6009,15 @@
       <c r="B8" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="133" t="s">
+      <c r="C8" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="134"/>
-      <c r="E8" s="134"/>
-      <c r="F8" s="134"/>
-      <c r="G8" s="134"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="135"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="139"/>
       <c r="M8" s="51"/>
       <c r="N8" s="51"/>
       <c r="O8" s="51"/>
@@ -6027,15 +6028,15 @@
       <c r="B9" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="122" t="s">
+      <c r="C9" s="126" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="124"/>
+      <c r="D9" s="127"/>
+      <c r="E9" s="127"/>
+      <c r="F9" s="127"/>
+      <c r="G9" s="127"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="128"/>
       <c r="M9" s="51"/>
       <c r="N9" s="51"/>
       <c r="O9" s="51"/>
@@ -6060,15 +6061,15 @@
       <c r="B11" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="119" t="s">
+      <c r="C11" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="121"/>
+      <c r="D11" s="124"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
+      <c r="G11" s="124"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="125"/>
     </row>
     <row r="12" spans="2:37" ht="18" x14ac:dyDescent="0.25">
       <c r="C12" s="64"/>
@@ -6890,11 +6891,11 @@
     </row>
     <row r="2" spans="2:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:4" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="37"/>
@@ -7950,25 +7951,49 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<p:Policy xmlns:p="office.server.policy" id="" local="true">
-  <p:Name>02 Departmental document</p:Name>
-  <p:Description/>
-  <p:Statement/>
-  <p:PolicyItems>
-    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.PolicyLabel">
-      <p:Name>Labels</p:Name>
-      <p:Description>Generates labels that can be inserted in Microsoft Office documents to ensure that document properties or other important information are included when documents are printed. Labels can also be used to search for documents.</p:Description>
-      <p:CustomData>
-        <label>
-          <segment type="metadata">_UIVersionString</segment>
-          <segment type="literal">\n</segment>
-          <segment type="metadata">_ModerationStatus</segment>
-        </label>
-      </p:CustomData>
-    </p:PolicyItem>
-  </p:PolicyItems>
-</p:Policy>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <View_x0020_CRM xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_CRM>
+    <View_x0020_Qua xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Qua>
+    <Document_x0020_author xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
+      <UserInfo>
+        <DisplayName>Jacobs, Frans</DisplayName>
+        <AccountId>1</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </Document_x0020_author>
+    <Document_x0020_type xmlns="5db227b6-3c56-4158-ad71-bd648583e357">Template</Document_x0020_type>
+    <View_x0020_Eng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_Eng>
+    <View_x0020_Production xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</View_x0020_Production>
+    <Relevant_x0020_to_x0020_ISO_x0020_13485 xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Relevant_x0020_to_x0020_ISO_x0020_13485>
+    <PInS_x0020_department xmlns="5db227b6-3c56-4158-ad71-bd648583e357">140 Software</PInS_x0020_department>
+    <Doc_x0020_nr. xmlns="5db227b6-3c56-4158-ad71-bd648583e357">BMS-REA-719</Doc_x0020_nr.>
+    <DLCPolicyLabelLock xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a" xsi:nil="true"/>
+    <Linked_x0020_to_x0020_PQRS xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</Linked_x0020_to_x0020_PQRS>
+    <Safety_x0020_relevant xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Safety_x0020_relevant>
+    <Approver xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
+      <UserInfo>
+        <DisplayName>Jacobs, Frans</DisplayName>
+        <AccountId>1</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </Approver>
+    <Reviewers xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Reviewers>
+    <Process xmlns="5db227b6-3c56-4158-ad71-bd648583e357">04 Realisation</Process>
+    <View_x0020_PL xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_PL>
+    <View_x0020_Mng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Mng>
+    <DLCPolicyLabelClientValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">{_UIVersionString}
+{_ModerationStatus}</DLCPolicyLabelClientValue>
+    <DLCPolicyLabelValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">1.0
+Approved</DLCPolicyLabelValue>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8362,49 +8387,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <View_x0020_CRM xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_CRM>
-    <View_x0020_Qua xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Qua>
-    <Document_x0020_author xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
-      <UserInfo>
-        <DisplayName>Jacobs, Frans</DisplayName>
-        <AccountId>1</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </Document_x0020_author>
-    <Document_x0020_type xmlns="5db227b6-3c56-4158-ad71-bd648583e357">Template</Document_x0020_type>
-    <View_x0020_Eng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_Eng>
-    <View_x0020_Production xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</View_x0020_Production>
-    <Relevant_x0020_to_x0020_ISO_x0020_13485 xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Relevant_x0020_to_x0020_ISO_x0020_13485>
-    <PInS_x0020_department xmlns="5db227b6-3c56-4158-ad71-bd648583e357">140 Software</PInS_x0020_department>
-    <Doc_x0020_nr. xmlns="5db227b6-3c56-4158-ad71-bd648583e357">BMS-REA-719</Doc_x0020_nr.>
-    <DLCPolicyLabelLock xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a" xsi:nil="true"/>
-    <Linked_x0020_to_x0020_PQRS xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</Linked_x0020_to_x0020_PQRS>
-    <Safety_x0020_relevant xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Safety_x0020_relevant>
-    <Approver xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
-      <UserInfo>
-        <DisplayName>Jacobs, Frans</DisplayName>
-        <AccountId>1</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </Approver>
-    <Reviewers xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Reviewers>
-    <Process xmlns="5db227b6-3c56-4158-ad71-bd648583e357">04 Realisation</Process>
-    <View_x0020_PL xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_PL>
-    <View_x0020_Mng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Mng>
-    <DLCPolicyLabelClientValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">{_UIVersionString}
-{_ModerationStatus}</DLCPolicyLabelClientValue>
-    <DLCPolicyLabelValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">1.0
-Approved</DLCPolicyLabelValue>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<p:Policy xmlns:p="office.server.policy" id="" local="true">
+  <p:Name>02 Departmental document</p:Name>
+  <p:Description/>
+  <p:Statement/>
+  <p:PolicyItems>
+    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.PolicyLabel">
+      <p:Name>Labels</p:Name>
+      <p:Description>Generates labels that can be inserted in Microsoft Office documents to ensure that document properties or other important information are included when documents are printed. Labels can also be used to search for documents.</p:Description>
+      <p:CustomData>
+        <label>
+          <segment type="metadata">_UIVersionString</segment>
+          <segment type="literal">\n</segment>
+          <segment type="metadata">_ModerationStatus</segment>
+        </label>
+      </p:CustomData>
+    </p:PolicyItem>
+  </p:PolicyItems>
+</p:Policy>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8417,9 +8418,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E0ECFB5-0E65-4944-A2C3-A12752EA8F83}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1320B1-D764-4C81-9B48-5F60482C3805}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="office.server.policy"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="5db227b6-3c56-4158-ad71-bd648583e357"/>
+    <ds:schemaRef ds:uri="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8444,18 +8454,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1320B1-D764-4C81-9B48-5F60482C3805}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E0ECFB5-0E65-4944-A2C3-A12752EA8F83}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5db227b6-3c56-4158-ad71-bd648583e357"/>
-    <ds:schemaRef ds:uri="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="office.server.policy"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update to Residual Anomalies document (one issue became a minor, discussed with Joost)
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_CommLib_Android_JaiVis-20161118-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_CommLib_Android_JaiVis-20161118-01V01.xlsx
@@ -1116,7 +1116,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1303,6 +1303,28 @@
     <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1371,29 +1393,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1584,13 +1583,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1612,6 +1604,13 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2437,7 +2436,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:F10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:F10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="B6:F10"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Version" dataDxfId="4"/>
@@ -2793,11 +2792,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="94"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -2863,10 +2862,10 @@
       <c r="C12" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="95"/>
+      <c r="E12" s="105"/>
       <c r="F12" s="28" t="s">
         <v>16</v>
       </c>
@@ -2881,10 +2880,10 @@
       <c r="C13" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="96"/>
+      <c r="E13" s="106"/>
       <c r="F13" s="28" t="s">
         <v>17</v>
       </c>
@@ -2899,8 +2898,8 @@
       <c r="C14" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="106"/>
       <c r="F14" s="28" t="s">
         <v>18</v>
       </c>
@@ -3028,11 +3027,11 @@
       <c r="C6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="103" t="s">
+      <c r="D6" s="113" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="104"/>
-      <c r="F6" s="105"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="115"/>
     </row>
     <row r="7" spans="2:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="30" t="s">
@@ -3041,11 +3040,11 @@
       <c r="C7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="106" t="s">
+      <c r="D7" s="116" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
     </row>
     <row r="8" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="31" t="s">
@@ -3097,27 +3096,27 @@
       <c r="D12" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="107" t="s">
+      <c r="E12" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="107"/>
+      <c r="F12" s="117"/>
     </row>
     <row r="13" spans="2:6" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="31"/>
       <c r="D13" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="97" t="s">
+      <c r="E13" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="98"/>
+      <c r="F13" s="108"/>
     </row>
     <row r="14" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="32"/>
       <c r="C14" s="30"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="99"/>
-      <c r="F14" s="100"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="110"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
@@ -3130,8 +3129,8 @@
       <c r="B16" s="19"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="102"/>
+      <c r="E16" s="111"/>
+      <c r="F16" s="112"/>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="48"/>
@@ -3310,19 +3309,19 @@
       <c r="N6" s="17"/>
     </row>
     <row r="7" spans="2:14" ht="28" x14ac:dyDescent="0.15">
-      <c r="B7" s="126" t="s">
+      <c r="B7" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="126" t="s">
+      <c r="C7" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="126" t="s">
+      <c r="D7" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="126" t="s">
+      <c r="E7" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="126" t="s">
+      <c r="F7" s="94" t="s">
         <v>72</v>
       </c>
       <c r="G7" s="17"/>
@@ -3335,19 +3334,19 @@
       <c r="N7" s="17"/>
     </row>
     <row r="8" spans="2:14" ht="14" x14ac:dyDescent="0.15">
-      <c r="B8" s="129" t="s">
+      <c r="B8" s="97" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="128" t="s">
+      <c r="C8" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="128" t="s">
+      <c r="D8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="129" t="s">
+      <c r="E8" s="97" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="129" t="s">
+      <c r="F8" s="97" t="s">
         <v>78</v>
       </c>
       <c r="G8" s="90"/>
@@ -3360,19 +3359,19 @@
       <c r="N8" s="17"/>
     </row>
     <row r="9" spans="2:14" ht="14" x14ac:dyDescent="0.15">
-      <c r="B9" s="127" t="s">
+      <c r="B9" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="128" t="s">
+      <c r="C9" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="128" t="s">
+      <c r="D9" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="129" t="s">
+      <c r="E9" s="97" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="129" t="s">
+      <c r="F9" s="97" t="s">
         <v>82</v>
       </c>
       <c r="G9" s="90"/>
@@ -3385,19 +3384,19 @@
       <c r="N9" s="17"/>
     </row>
     <row r="10" spans="2:14" ht="14" x14ac:dyDescent="0.15">
-      <c r="B10" s="132" t="s">
+      <c r="B10" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="130" t="s">
+      <c r="C10" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="130" t="s">
+      <c r="D10" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="131" t="s">
+      <c r="E10" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="131" t="s">
+      <c r="F10" s="99" t="s">
         <v>89</v>
       </c>
       <c r="G10" s="89"/>
@@ -6071,19 +6070,19 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:37" ht="120.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="114" t="s">
+      <c r="B4" s="124" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="125"/>
+      <c r="J4" s="125"/>
+      <c r="K4" s="125"/>
+      <c r="L4" s="125"/>
     </row>
     <row r="5" spans="2:37" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="45"/>
@@ -6102,29 +6101,29 @@
       <c r="B6" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="117"/>
-      <c r="I6" s="118"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="128"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B7" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="119" t="s">
+      <c r="C7" s="129" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="120"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="121"/>
+      <c r="D7" s="130"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="131"/>
       <c r="M7" s="51"/>
       <c r="N7" s="51"/>
       <c r="O7" s="51"/>
@@ -6135,15 +6134,15 @@
       <c r="B8" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="132" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="123"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="124"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
+      <c r="H8" s="133"/>
+      <c r="I8" s="134"/>
       <c r="M8" s="51"/>
       <c r="N8" s="51"/>
       <c r="O8" s="51"/>
@@ -6154,15 +6153,15 @@
       <c r="B9" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="111" t="s">
+      <c r="C9" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="113"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="122"/>
+      <c r="I9" s="123"/>
       <c r="M9" s="51"/>
       <c r="N9" s="51"/>
       <c r="O9" s="51"/>
@@ -6187,15 +6186,15 @@
       <c r="B11" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="108" t="s">
+      <c r="C11" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="109"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="110"/>
+      <c r="D11" s="119"/>
+      <c r="E11" s="119"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="119"/>
+      <c r="H11" s="119"/>
+      <c r="I11" s="120"/>
     </row>
     <row r="12" spans="2:37" ht="18" x14ac:dyDescent="0.2">
       <c r="C12" s="64"/>
@@ -6300,7 +6299,7 @@
   <dimension ref="B1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7017,11 +7016,11 @@
     </row>
     <row r="2" spans="2:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="2:4" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="37"/>
@@ -7051,7 +7050,7 @@
         <v>49</v>
       </c>
       <c r="C7" s="80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="37"/>
     </row>
@@ -7060,7 +7059,7 @@
         <v>50</v>
       </c>
       <c r="C8" s="82">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="37"/>
     </row>
@@ -7114,7 +7113,7 @@
   <dimension ref="B1:AH29"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="120" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7848,13 +7847,13 @@
       <c r="AH3" s="34"/>
     </row>
     <row r="4" spans="2:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="134" t="s">
+      <c r="C4" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="135"/>
+      <c r="D4" s="103"/>
       <c r="AD4" s="34"/>
       <c r="AE4" s="34"/>
       <c r="AF4" s="34"/>
@@ -7862,10 +7861,10 @@
       <c r="AH4" s="34"/>
     </row>
     <row r="5" spans="2:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="101" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="134" t="s">
+      <c r="C5" s="102" t="s">
         <v>93</v>
       </c>
       <c r="D5" s="71" t="s">
@@ -7878,10 +7877,10 @@
       <c r="AH5" s="34"/>
     </row>
     <row r="6" spans="2:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="133" t="s">
+      <c r="B6" s="101" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C6" s="102" t="s">
         <v>95</v>
       </c>
       <c r="D6" s="71" t="s">
@@ -7894,10 +7893,10 @@
       <c r="AH6" s="34"/>
     </row>
     <row r="7" spans="2:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="133" t="s">
+      <c r="B7" s="101" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="134" t="s">
+      <c r="C7" s="102" t="s">
         <v>97</v>
       </c>
       <c r="D7" s="71" t="s">
@@ -7910,10 +7909,10 @@
       <c r="AH7" s="34"/>
     </row>
     <row r="8" spans="2:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="133" t="s">
+      <c r="B8" s="101" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="134" t="s">
+      <c r="C8" s="102" t="s">
         <v>99</v>
       </c>
       <c r="D8" s="71" t="s">
@@ -7926,14 +7925,14 @@
       <c r="AH8" s="34"/>
     </row>
     <row r="9" spans="2:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="133" t="s">
+      <c r="B9" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="134" t="s">
+      <c r="C9" s="102" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="136" t="s">
-        <v>49</v>
+      <c r="D9" s="71" t="s">
+        <v>50</v>
       </c>
       <c r="AD9" s="34"/>
       <c r="AE9" s="34"/>
@@ -7942,13 +7941,13 @@
       <c r="AH9" s="34"/>
     </row>
     <row r="10" spans="2:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="133" t="s">
+      <c r="B10" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="134" t="s">
+      <c r="C10" s="102" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="135"/>
+      <c r="D10" s="103"/>
       <c r="AD10" s="34"/>
       <c r="AE10" s="34"/>
       <c r="AF10" s="34"/>
@@ -7956,13 +7955,13 @@
       <c r="AH10" s="34"/>
     </row>
     <row r="11" spans="2:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="133" t="s">
+      <c r="B11" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="134" t="s">
+      <c r="C11" s="102" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="135"/>
+      <c r="D11" s="103"/>
       <c r="AD11" s="34"/>
       <c r="AE11" s="34"/>
       <c r="AF11" s="34"/>
@@ -7970,13 +7969,13 @@
       <c r="AH11" s="34"/>
     </row>
     <row r="12" spans="2:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="133" t="s">
+      <c r="B12" s="101" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="134" t="s">
+      <c r="C12" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="135"/>
+      <c r="D12" s="103"/>
       <c r="AD12" s="34"/>
       <c r="AE12" s="34"/>
       <c r="AF12" s="34"/>
@@ -8084,52 +8083,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <View_x0020_CRM xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_CRM>
-    <View_x0020_Qua xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Qua>
-    <Document_x0020_author xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
-      <UserInfo>
-        <DisplayName>Jacobs, Frans</DisplayName>
-        <AccountId>1</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </Document_x0020_author>
-    <Document_x0020_type xmlns="5db227b6-3c56-4158-ad71-bd648583e357">Template</Document_x0020_type>
-    <View_x0020_Eng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_Eng>
-    <View_x0020_Production xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</View_x0020_Production>
-    <Relevant_x0020_to_x0020_ISO_x0020_13485 xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Relevant_x0020_to_x0020_ISO_x0020_13485>
-    <PInS_x0020_department xmlns="5db227b6-3c56-4158-ad71-bd648583e357">140 Software</PInS_x0020_department>
-    <Doc_x0020_nr. xmlns="5db227b6-3c56-4158-ad71-bd648583e357">BMS-REA-719</Doc_x0020_nr.>
-    <DLCPolicyLabelLock xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a" xsi:nil="true"/>
-    <Linked_x0020_to_x0020_PQRS xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</Linked_x0020_to_x0020_PQRS>
-    <Safety_x0020_relevant xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Safety_x0020_relevant>
-    <Approver xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
-      <UserInfo>
-        <DisplayName>Jacobs, Frans</DisplayName>
-        <AccountId>1</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </Approver>
-    <Reviewers xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Reviewers>
-    <Process xmlns="5db227b6-3c56-4158-ad71-bd648583e357">04 Realisation</Process>
-    <View_x0020_PL xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_PL>
-    <View_x0020_Mng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Mng>
-    <DLCPolicyLabelClientValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">{_UIVersionString}
-{_ModerationStatus}</DLCPolicyLabelClientValue>
-    <DLCPolicyLabelValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">1.0
-Approved</DLCPolicyLabelValue>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="02 Departmental document" ma:contentTypeID="0x0101001E9AF57F6A6FB1498E6BAB1704371DB9020048B3E13A56EC2B4880B8E17388254DB6" ma:contentTypeVersion="42" ma:contentTypeDescription="A document under departmental control" ma:contentTypeScope="" ma:versionID="28e15f56482d8af7e67347cbef2a0996">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5db227b6-3c56-4158-ad71-bd648583e357" xmlns:ns3="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa83b77159cc0e9c22a0bfa7b50ba950" ns2:_="" ns3:_="">
     <xsd:import namespace="5db227b6-3c56-4158-ad71-bd648583e357"/>
@@ -8519,7 +8472,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <p:Policy xmlns:p="office.server.policy" id="" local="true">
   <p:Name>02 Departmental document</p:Name>
@@ -8541,7 +8494,7 @@
 </p:Policy>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8550,24 +8503,53 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1320B1-D764-4C81-9B48-5F60482C3805}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5db227b6-3c56-4158-ad71-bd648583e357"/>
-    <ds:schemaRef ds:uri="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <View_x0020_CRM xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_CRM>
+    <View_x0020_Qua xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Qua>
+    <Document_x0020_author xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
+      <UserInfo>
+        <DisplayName>Jacobs, Frans</DisplayName>
+        <AccountId>1</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </Document_x0020_author>
+    <Document_x0020_type xmlns="5db227b6-3c56-4158-ad71-bd648583e357">Template</Document_x0020_type>
+    <View_x0020_Eng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_Eng>
+    <View_x0020_Production xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</View_x0020_Production>
+    <Relevant_x0020_to_x0020_ISO_x0020_13485 xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Relevant_x0020_to_x0020_ISO_x0020_13485>
+    <PInS_x0020_department xmlns="5db227b6-3c56-4158-ad71-bd648583e357">140 Software</PInS_x0020_department>
+    <Doc_x0020_nr. xmlns="5db227b6-3c56-4158-ad71-bd648583e357">BMS-REA-719</Doc_x0020_nr.>
+    <DLCPolicyLabelLock xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a" xsi:nil="true"/>
+    <Linked_x0020_to_x0020_PQRS xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">false</Linked_x0020_to_x0020_PQRS>
+    <Safety_x0020_relevant xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</Safety_x0020_relevant>
+    <Approver xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
+      <UserInfo>
+        <DisplayName>Jacobs, Frans</DisplayName>
+        <AccountId>1</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </Approver>
+    <Reviewers xmlns="5db227b6-3c56-4158-ad71-bd648583e357">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Reviewers>
+    <Process xmlns="5db227b6-3c56-4158-ad71-bd648583e357">04 Realisation</Process>
+    <View_x0020_PL xmlns="5db227b6-3c56-4158-ad71-bd648583e357">true</View_x0020_PL>
+    <View_x0020_Mng xmlns="5db227b6-3c56-4158-ad71-bd648583e357">false</View_x0020_Mng>
+    <DLCPolicyLabelClientValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">{_UIVersionString}
+{_ModerationStatus}</DLCPolicyLabelClientValue>
+    <DLCPolicyLabelValue xmlns="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a">1.0
+Approved</DLCPolicyLabelValue>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3331877D-A973-4A26-8E19-E1DD744074D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8586,7 +8568,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E0ECFB5-0E65-4944-A2C3-A12752EA8F83}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="office.server.policy"/>
@@ -8594,10 +8576,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F20991C-9C75-4A23-AD56-83877EA734AB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1320B1-D764-4C81-9B48-5F60482C3805}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="5db227b6-3c56-4158-ad71-bd648583e357"/>
+    <ds:schemaRef ds:uri="ce34623b-5c11-4b5b-b0d3-7d70f0a3097a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>